<commit_message>
modified:   example_output/database/consulting_firm.db 	modified:   example_output/spreadsheets/indirect_costs.xlsx 	modified:   example_output/spreadsheets/non_billable_time.xlsx 	modified:   requirements.txt 	modified:   src/config/project_settings.py 	modified:   src/database_generator/generators/project_deliverable.py 	modified:   src/database_generator/utils/project_financial_utils.py 	modified:   src/database_generator/utils/project_utils.py 	modified:   src/etl_service/sqlite_to_snowflake.py 	modified:   src/main.py
</commit_message>
<xml_diff>
--- a/example_output/spreadsheets/indirect_costs.xlsx
+++ b/example_output/spreadsheets/indirect_costs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -669,6 +669,234 @@
         <v>321210.78</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Dec-15</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>258650.74</v>
+      </c>
+      <c r="D13" t="n">
+        <v>55717.72</v>
+      </c>
+      <c r="E13" t="n">
+        <v>314368.46</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Jan-16</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>252175.98</v>
+      </c>
+      <c r="D14" t="n">
+        <v>58329.03</v>
+      </c>
+      <c r="E14" t="n">
+        <v>310505.01</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Feb-16</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>244305.23</v>
+      </c>
+      <c r="D15" t="n">
+        <v>60012.48</v>
+      </c>
+      <c r="E15" t="n">
+        <v>304317.71</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mar-16</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>241621.2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>58528.24</v>
+      </c>
+      <c r="E16" t="n">
+        <v>300149.44</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Apr-16</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>239032.88</v>
+      </c>
+      <c r="D17" t="n">
+        <v>63694.36</v>
+      </c>
+      <c r="E17" t="n">
+        <v>302727.24</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>May-16</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>239635.18</v>
+      </c>
+      <c r="D18" t="n">
+        <v>57655.44</v>
+      </c>
+      <c r="E18" t="n">
+        <v>297290.62</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Jun-16</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>243293.68</v>
+      </c>
+      <c r="D19" t="n">
+        <v>54036.96</v>
+      </c>
+      <c r="E19" t="n">
+        <v>297330.64</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Jul-16</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>242000.98</v>
+      </c>
+      <c r="D20" t="n">
+        <v>50080.31</v>
+      </c>
+      <c r="E20" t="n">
+        <v>292081.29</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Aug-16</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>234265.6</v>
+      </c>
+      <c r="D21" t="n">
+        <v>54302.69</v>
+      </c>
+      <c r="E21" t="n">
+        <v>288568.29</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Sep-16</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>240823.88</v>
+      </c>
+      <c r="D22" t="n">
+        <v>56481.26</v>
+      </c>
+      <c r="E22" t="n">
+        <v>297305.14</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Oct-16</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>240985.37</v>
+      </c>
+      <c r="D23" t="n">
+        <v>56440.75</v>
+      </c>
+      <c r="E23" t="n">
+        <v>297426.12</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Nov-16</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>235683.88</v>
+      </c>
+      <c r="D24" t="n">
+        <v>55490.59</v>
+      </c>
+      <c r="E24" t="n">
+        <v>291174.47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>